<commit_message>
- codigo do sensor de temperatura - implementacao da leitura da temperatura pelo painel de controle - correcoes de problemas gerais (eletricos)
</commit_message>
<xml_diff>
--- a/tabela comandos.xlsx
+++ b/tabela comandos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Caio\UFSCar\Laboratório de microcontroladores\projetoFinal\ProjetoFinalMic.git\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>CMD</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>caractere</t>
+  </si>
+  <si>
+    <t>ler valor da temperatura</t>
+  </si>
+  <si>
+    <t>temp atual</t>
   </si>
 </sst>
 </file>
@@ -419,7 +425,7 @@
   <dimension ref="C2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +433,7 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="86.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
@@ -594,10 +601,16 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>127</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>

</xml_diff>